<commit_message>
chasing down issues with SLR-045A
</commit_message>
<xml_diff>
--- a/0 - Field Data Sheets/Weir Calibration Field Form 2019 CURRENT 07_31_2019.xlsx
+++ b/0 - Field Data Sheets/Weir Calibration Field Form 2019 CURRENT 07_31_2019.xlsx
@@ -17,7 +17,7 @@
     <sheet name="ESRI_MAPINFO_SHEET" sheetId="3" state="veryHidden" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Form Responses 1'!$A$1:$U$350</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Form Responses 1'!$A$1:$U$454</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -1961,7 +1961,7 @@
         <xdr:cNvPr id="2" name="EsriDoNotEdit">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2304,14 +2304,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:W454"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A445" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A454" sqref="A454:XFD454"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A311" sqref="A311:XFD314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2385,7 +2385,7 @@
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
     </row>
-    <row r="2" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>43588.755538854166</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>3050</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>43588.760185335646</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>43588.762669606484</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>5900</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>43591.435261481485</v>
       </c>
@@ -2504,7 +2504,7 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>43591.44535303241</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>11400</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>43591.464841817127</v>
       </c>
@@ -2568,7 +2568,7 @@
         <v>5200</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>43591.470591574078</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>43591.472597476852</v>
       </c>
@@ -2632,7 +2632,7 @@
         <v>4200</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>43591.479208553239</v>
       </c>
@@ -2664,7 +2664,7 @@
         <v>5600</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>43591.485304733797</v>
       </c>
@@ -2696,7 +2696,7 @@
         <v>4200</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>43591.492769594908</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>8200</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>43591.502019652777</v>
       </c>
@@ -2760,7 +2760,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>43591.512494085648</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>43591.521164178237</v>
       </c>
@@ -2824,7 +2824,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>43591.527513136578</v>
       </c>
@@ -2856,7 +2856,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>43591.537957824075</v>
       </c>
@@ -2888,7 +2888,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>43591.548731967589</v>
       </c>
@@ -2920,7 +2920,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>43591.560089768522</v>
       </c>
@@ -2952,7 +2952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>43591.572355104166</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>43591.577724270828</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>43591.58141392361</v>
       </c>
@@ -3045,7 +3045,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>43591.583598541663</v>
       </c>
@@ -3123,7 +3123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>43591.704277094905</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>43591.755216921301</v>
       </c>
@@ -3163,7 +3163,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>43591.757524560184</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>43591.775486631945</v>
       </c>
@@ -3203,7 +3203,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>43591.776427210643</v>
       </c>
@@ -3226,7 +3226,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>43592.481644421292</v>
       </c>
@@ -3255,7 +3255,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>43592.482017627313</v>
       </c>
@@ -3284,7 +3284,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>43592.50501202546</v>
       </c>
@@ -3316,7 +3316,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <v>43592.532280358791</v>
       </c>
@@ -3348,7 +3348,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>43592.545401550931</v>
       </c>
@@ -3389,7 +3389,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>43592.637291597217</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>14200</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>43592.563986909721</v>
       </c>
@@ -3465,7 +3465,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>43592.580991099538</v>
       </c>
@@ -3497,7 +3497,7 @@
         <v>3100</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>43592.581140219903</v>
       </c>
@@ -3541,7 +3541,7 @@
         <v>4480</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <v>43592.640366712963</v>
       </c>
@@ -3573,7 +3573,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>43592.657211875005</v>
       </c>
@@ -3605,7 +3605,7 @@
         <v>4090</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <v>43592.681611643522</v>
       </c>
@@ -3632,7 +3632,7 @@
       </c>
       <c r="J42" s="5"/>
     </row>
-    <row r="43" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>43592.691540694446</v>
       </c>
@@ -3676,7 +3676,7 @@
         <v>2375</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <v>43592.702423842595</v>
       </c>
@@ -3720,7 +3720,7 @@
         <v>1560</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
         <v>43593.43748443287</v>
       </c>
@@ -3752,7 +3752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <v>43593.44123866898</v>
       </c>
@@ -3781,7 +3781,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <v>43593.460052071758</v>
       </c>
@@ -3825,7 +3825,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
         <v>43593.476238275463</v>
       </c>
@@ -3869,7 +3869,7 @@
         <v>1740</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <v>43593.518983738424</v>
       </c>
@@ -3913,7 +3913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <v>43593.527186284722</v>
       </c>
@@ -3942,7 +3942,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>43593.548600451388</v>
       </c>
@@ -3971,7 +3971,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
         <v>43593.553772789353</v>
       </c>
@@ -4015,7 +4015,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
         <v>43593.598725358795</v>
       </c>
@@ -4038,7 +4038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <v>43593.610852187499</v>
       </c>
@@ -4079,7 +4079,7 @@
         <v>6250</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
         <v>43593.612856157408</v>
       </c>
@@ -4120,7 +4120,7 @@
         <v>7580</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
         <v>43593.617690162035</v>
       </c>
@@ -4161,7 +4161,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="57" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7">
         <v>43593.618488009262</v>
       </c>
@@ -4184,7 +4184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
         <v>43593.619830208336</v>
       </c>
@@ -4225,7 +4225,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7">
         <v>43593.656584456017</v>
       </c>
@@ -4266,7 +4266,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="60" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
         <v>43593.658092847225</v>
       </c>
@@ -4310,7 +4310,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="61" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7">
         <v>43593.660192870375</v>
       </c>
@@ -4354,7 +4354,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
         <v>43593.6652215625</v>
       </c>
@@ -4398,7 +4398,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="7">
         <v>43593.691000405088</v>
       </c>
@@ -4418,7 +4418,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="64" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
         <v>43594.407145740741</v>
       </c>
@@ -4462,7 +4462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7">
         <v>43594.410411932869</v>
       </c>
@@ -4506,7 +4506,7 @@
         <v>2170</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="7">
         <v>43594.419389386574</v>
       </c>
@@ -4550,7 +4550,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
         <v>43594.424918101853</v>
       </c>
@@ -4594,7 +4594,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="7">
         <v>43594.431594340276</v>
       </c>
@@ -4626,7 +4626,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="7">
         <v>43594.432673472227</v>
       </c>
@@ -4670,7 +4670,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="7">
         <v>43594.435762604167</v>
       </c>
@@ -4714,7 +4714,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="7">
         <v>43594.444414444442</v>
       </c>
@@ -4758,7 +4758,7 @@
         <v>2460</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="7">
         <v>43594.445713379631</v>
       </c>
@@ -4790,7 +4790,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="73" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="7">
         <v>43594.461393437501</v>
       </c>
@@ -4822,7 +4822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="7">
         <v>43594.467428356482</v>
       </c>
@@ -4866,7 +4866,7 @@
         <v>5570</v>
       </c>
     </row>
-    <row r="75" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="7">
         <v>43594.491857604167</v>
       </c>
@@ -4910,7 +4910,7 @@
         <v>4680</v>
       </c>
     </row>
-    <row r="76" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="7">
         <v>43594.514163171298</v>
       </c>
@@ -4942,7 +4942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="7">
         <v>43594.530017488425</v>
       </c>
@@ -4986,7 +4986,7 @@
         <v>2670</v>
       </c>
     </row>
-    <row r="78" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="7">
         <v>43594.584730694449</v>
       </c>
@@ -5009,7 +5009,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="7">
         <v>43594.611498634258</v>
       </c>
@@ -5035,7 +5035,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="80" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="7">
         <v>43594.624838090276</v>
       </c>
@@ -5079,7 +5079,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="81" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="7">
         <v>43594.648807557867</v>
       </c>
@@ -5123,7 +5123,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="82" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="7">
         <v>43594.653585208333</v>
       </c>
@@ -5152,7 +5152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="7">
         <v>43594.667883368056</v>
       </c>
@@ -5178,7 +5178,7 @@
         <v>-1.4</v>
       </c>
     </row>
-    <row r="84" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="7">
         <v>43594.676933946757</v>
       </c>
@@ -5198,7 +5198,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="85" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="7">
         <v>43594.68904351852</v>
       </c>
@@ -5242,7 +5242,7 @@
         <v>3890</v>
       </c>
     </row>
-    <row r="86" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="7">
         <v>43594.893515358795</v>
       </c>
@@ -5374,7 +5374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="7">
         <v>43594.89877886574</v>
       </c>
@@ -5418,7 +5418,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="90" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="7">
         <v>43594.900322071757</v>
       </c>
@@ -5459,7 +5459,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="91" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="7">
         <v>43594.901593657407</v>
       </c>
@@ -5500,7 +5500,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="92" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="7">
         <v>43594.903644548613</v>
       </c>
@@ -5541,7 +5541,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="93" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="7">
         <v>43594.905283796295</v>
       </c>
@@ -5582,7 +5582,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="94" spans="1:15" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="7">
         <v>43594.907106331018</v>
       </c>
@@ -5626,7 +5626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="7">
         <v>43594.908273356486</v>
       </c>
@@ -5667,7 +5667,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="96" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="7">
         <v>43594.909638333338</v>
       </c>
@@ -5708,7 +5708,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="97" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="7">
         <v>43594.91069650463</v>
       </c>
@@ -5749,7 +5749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="7">
         <v>43594.912148344913</v>
       </c>
@@ -5790,7 +5790,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="99" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="7">
         <v>43594.913895949074</v>
       </c>
@@ -5831,7 +5831,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="100" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="7">
         <v>43595.442240902776</v>
       </c>
@@ -5851,7 +5851,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="101" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="7">
         <v>43595.448872152774</v>
       </c>
@@ -5892,7 +5892,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="102" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="7">
         <v>43595.470052662036</v>
       </c>
@@ -5997,7 +5997,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="105" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="7">
         <v>43595.474870532409</v>
       </c>
@@ -6041,7 +6041,7 @@
         <v>2980</v>
       </c>
     </row>
-    <row r="106" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="7">
         <v>43595.481380717596</v>
       </c>
@@ -6076,7 +6076,7 @@
         <v>7030</v>
       </c>
     </row>
-    <row r="107" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="7">
         <v>43595.490416296292</v>
       </c>
@@ -6117,7 +6117,7 @@
         <v>6300</v>
       </c>
     </row>
-    <row r="108" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="7">
         <v>43595.500877777777</v>
       </c>
@@ -6155,7 +6155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="7">
         <v>43595.509428749996</v>
       </c>
@@ -6190,7 +6190,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="110" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="7">
         <v>43595.513097534727</v>
       </c>
@@ -6234,7 +6234,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="111" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="7">
         <v>43595.516432615739</v>
       </c>
@@ -6275,7 +6275,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="112" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="7">
         <v>43595.524782893517</v>
       </c>
@@ -6319,7 +6319,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="113" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="7">
         <v>43595.537118668981</v>
       </c>
@@ -6363,7 +6363,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="114" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="7">
         <v>43595.554605081023</v>
       </c>
@@ -6386,7 +6386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="7">
         <v>43595.554936168977</v>
       </c>
@@ -6409,7 +6409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="7">
         <v>43595.556602696757</v>
       </c>
@@ -6432,7 +6432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="7">
         <v>43595.5592850463</v>
       </c>
@@ -6455,7 +6455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="7">
         <v>43595.568305081018</v>
       </c>
@@ -6490,7 +6490,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="119" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="7">
         <v>43595.569374467595</v>
       </c>
@@ -6531,7 +6531,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="120" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="7">
         <v>43595.586062511575</v>
       </c>
@@ -6566,7 +6566,7 @@
         <v>2650</v>
       </c>
     </row>
-    <row r="121" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="7">
         <v>43595.587130358792</v>
       </c>
@@ -6601,7 +6601,7 @@
         <v>2430</v>
       </c>
     </row>
-    <row r="122" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="7">
         <v>43595.588972465281</v>
       </c>
@@ -6636,7 +6636,7 @@
         <v>2430</v>
       </c>
     </row>
-    <row r="123" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="7">
         <v>43595.590072256949</v>
       </c>
@@ -6671,7 +6671,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="124" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="7">
         <v>43595.594992129627</v>
       </c>
@@ -6715,7 +6715,7 @@
         <v>1230</v>
       </c>
     </row>
-    <row r="125" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="7">
         <v>43595.619344803243</v>
       </c>
@@ -6759,7 +6759,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="126" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="7">
         <v>43595.663596446757</v>
       </c>
@@ -6794,7 +6794,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="127" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="7">
         <v>43595.682554699073</v>
       </c>
@@ -6835,7 +6835,7 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="128" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="7">
         <v>43595.689118402777</v>
       </c>
@@ -6870,7 +6870,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="129" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="7">
         <v>43595.691901261569</v>
       </c>
@@ -6890,7 +6890,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="130" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="7">
         <v>43595.693264699075</v>
       </c>
@@ -6919,7 +6919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="7">
         <v>43595.707292939813</v>
       </c>
@@ -6948,7 +6948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="7">
         <v>43595.708949965279</v>
       </c>
@@ -6977,7 +6977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="7">
         <v>43595.711790578702</v>
       </c>
@@ -7006,7 +7006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="7">
         <v>43595.725159085647</v>
       </c>
@@ -7029,7 +7029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="7">
         <v>43598.523171504625</v>
       </c>
@@ -7073,7 +7073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="7">
         <v>43598.531430370371</v>
       </c>
@@ -7117,7 +7117,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="137" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="7">
         <v>43598.538723784717</v>
       </c>
@@ -7161,7 +7161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="7">
         <v>43598.55321135417</v>
       </c>
@@ -7205,7 +7205,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="139" spans="1:15" s="11" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:15" s="11" customFormat="1" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="10">
         <v>43598.558324872683</v>
       </c>
@@ -7234,7 +7234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="7">
         <v>43598.568272129633</v>
       </c>
@@ -7278,7 +7278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="7">
         <v>43598.660832187496</v>
       </c>
@@ -7322,7 +7322,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="142" spans="1:15" s="11" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:15" s="11" customFormat="1" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="10">
         <v>43598.669797893519</v>
       </c>
@@ -7354,7 +7354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="7">
         <v>43599.412810810187</v>
       </c>
@@ -7395,7 +7395,7 @@
         <v>3260</v>
       </c>
     </row>
-    <row r="144" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="7">
         <v>43599.427670717589</v>
       </c>
@@ -7439,7 +7439,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="145" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="7">
         <v>43599.433456574072</v>
       </c>
@@ -7483,7 +7483,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="146" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="7">
         <v>43599.459267349535</v>
       </c>
@@ -7527,7 +7527,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="147" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="7">
         <v>43599.470011574071</v>
       </c>
@@ -7571,7 +7571,7 @@
         <v>2520</v>
       </c>
     </row>
-    <row r="148" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="7">
         <v>43599.485035810183</v>
       </c>
@@ -7597,7 +7597,7 @@
         <v>16.8</v>
       </c>
     </row>
-    <row r="149" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="7">
         <v>43599.500831736106</v>
       </c>
@@ -7623,7 +7623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="7">
         <v>43599.518437384264</v>
       </c>
@@ -7655,7 +7655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="7">
         <v>43599.539609108797</v>
       </c>
@@ -7699,7 +7699,7 @@
         <v>2380</v>
       </c>
     </row>
-    <row r="152" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="7">
         <v>43599.569834490743</v>
       </c>
@@ -7743,7 +7743,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="153" spans="1:15" s="11" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:15" s="11" customFormat="1" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="10">
         <v>43599.624617476853</v>
       </c>
@@ -7772,7 +7772,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="154" spans="1:15" s="11" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:15" s="11" customFormat="1" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="10">
         <v>43599.639232141199</v>
       </c>
@@ -7804,7 +7804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="7">
         <v>43599.738793206023</v>
       </c>
@@ -7848,7 +7848,7 @@
         <v>2160</v>
       </c>
     </row>
-    <row r="156" spans="1:15" s="11" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:15" s="11" customFormat="1" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="10">
         <v>43600.422265266199</v>
       </c>
@@ -7880,7 +7880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="7">
         <v>43600.482206006942</v>
       </c>
@@ -8000,7 +8000,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="160" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="7">
         <v>43600.528849884256</v>
       </c>
@@ -8044,7 +8044,7 @@
         <v>1450</v>
       </c>
     </row>
-    <row r="161" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="7">
         <v>43600.601932974532</v>
       </c>
@@ -8088,7 +8088,7 @@
         <v>2190</v>
       </c>
     </row>
-    <row r="162" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="7">
         <v>43600.638289583338</v>
       </c>
@@ -8132,7 +8132,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="163" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="7">
         <v>43600.686218657407</v>
       </c>
@@ -8176,7 +8176,7 @@
         <v>9850</v>
       </c>
     </row>
-    <row r="164" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="7">
         <v>43600.725389861109</v>
       </c>
@@ -8220,7 +8220,7 @@
         <v>3105</v>
       </c>
     </row>
-    <row r="165" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="7">
         <v>43601.407068912042</v>
       </c>
@@ -8255,7 +8255,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="166" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="7">
         <v>43601.40923740741</v>
       </c>
@@ -8278,7 +8278,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="167" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="7">
         <v>43601.414449374999</v>
       </c>
@@ -8301,7 +8301,7 @@
         <v>-1.3</v>
       </c>
     </row>
-    <row r="168" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="7">
         <v>43601.415471493056</v>
       </c>
@@ -8330,7 +8330,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="169" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="7">
         <v>43601.417819421295</v>
       </c>
@@ -8359,7 +8359,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="170" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="7">
         <v>43601.419731273148</v>
       </c>
@@ -8388,7 +8388,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="171" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="7">
         <v>43601.427588611114</v>
       </c>
@@ -8417,7 +8417,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="172" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="7">
         <v>43602.442062349539</v>
       </c>
@@ -8452,7 +8452,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="173" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="7">
         <v>43602.451806273151</v>
       </c>
@@ -8490,7 +8490,7 @@
         <v>1190</v>
       </c>
     </row>
-    <row r="174" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="7">
         <v>43602.47989505787</v>
       </c>
@@ -8516,7 +8516,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="175" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="7">
         <v>43602.489967141199</v>
       </c>
@@ -8554,7 +8554,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="176" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="7">
         <v>43602.509337268522</v>
       </c>
@@ -8592,7 +8592,7 @@
         <v>3700</v>
       </c>
     </row>
-    <row r="177" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="7">
         <v>43602.522517500001</v>
       </c>
@@ -8627,7 +8627,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="178" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="7">
         <v>43606.707793877315</v>
       </c>
@@ -8668,7 +8668,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="179" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="7">
         <v>43606.723546145833</v>
       </c>
@@ -8709,7 +8709,7 @@
         <v>1830</v>
       </c>
     </row>
-    <row r="180" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="7">
         <v>43608.481453252316</v>
       </c>
@@ -8738,7 +8738,7 @@
         <v>9100</v>
       </c>
     </row>
-    <row r="181" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="7">
         <v>43608.482445162037</v>
       </c>
@@ -8767,7 +8767,7 @@
         <v>8050</v>
       </c>
     </row>
-    <row r="182" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="7">
         <v>43608.483487696758</v>
       </c>
@@ -8796,7 +8796,7 @@
         <v>7240</v>
       </c>
     </row>
-    <row r="183" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:15" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="7">
         <v>43608.526771817131</v>
       </c>
@@ -8828,7 +8828,7 @@
         <v>3480</v>
       </c>
     </row>
-    <row r="184" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="7">
         <v>43619.387044270828</v>
       </c>
@@ -8851,7 +8851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="7">
         <v>43619.417066539347</v>
       </c>
@@ -8880,7 +8880,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="186" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="7">
         <v>43619.424325891203</v>
       </c>
@@ -8915,7 +8915,7 @@
         <v>8600</v>
       </c>
     </row>
-    <row r="187" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="7">
         <v>43619.430370590278</v>
       </c>
@@ -8944,7 +8944,7 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="188" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="7">
         <v>43619.448148344905</v>
       </c>
@@ -9055,7 +9055,7 @@
         <v>4910</v>
       </c>
     </row>
-    <row r="191" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="7">
         <v>43619.481042361112</v>
       </c>
@@ -9084,7 +9084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="7">
         <v>43619.482240219906</v>
       </c>
@@ -9113,7 +9113,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="193" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="7">
         <v>43619.485708449072</v>
       </c>
@@ -9142,7 +9142,7 @@
         <v>2470</v>
       </c>
     </row>
-    <row r="194" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="7">
         <v>43619.502512523148</v>
       </c>
@@ -9171,7 +9171,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="195" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="7">
         <v>43619.50333712963</v>
       </c>
@@ -9194,7 +9194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="7">
         <v>43619.512569479164</v>
       </c>
@@ -9223,7 +9223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="7">
         <v>43619.559027557872</v>
       </c>
@@ -9252,7 +9252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="7">
         <v>43619.560911979162</v>
       </c>
@@ -9275,7 +9275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="7">
         <v>43619.580106157402</v>
       </c>
@@ -9304,7 +9304,7 @@
         <v>8500</v>
       </c>
     </row>
-    <row r="200" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="7">
         <v>43619.586162476851</v>
       </c>
@@ -9327,7 +9327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="7">
         <v>43619.593100185186</v>
       </c>
@@ -9359,7 +9359,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="202" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="7">
         <v>43619.603138240738</v>
       </c>
@@ -9388,7 +9388,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="203" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="7">
         <v>43619.624149479168</v>
       </c>
@@ -9417,7 +9417,7 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="204" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="7">
         <v>43619.636075578703</v>
       </c>
@@ -9449,7 +9449,7 @@
         <v>2820</v>
       </c>
     </row>
-    <row r="205" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="7">
         <v>43619.657319212958</v>
       </c>
@@ -9481,7 +9481,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="206" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="7">
         <v>43619.669281388888</v>
       </c>
@@ -9504,7 +9504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="7">
         <v>43619.683368090278</v>
       </c>
@@ -9536,7 +9536,7 @@
         <v>2220</v>
       </c>
     </row>
-    <row r="208" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="7">
         <v>43620.42668315972</v>
       </c>
@@ -9562,7 +9562,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="209" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="7">
         <v>43620.433715914347</v>
       </c>
@@ -9591,7 +9591,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="210" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="7">
         <v>43620.449795451394</v>
       </c>
@@ -9620,7 +9620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="7">
         <v>43620.468617280094</v>
       </c>
@@ -9664,7 +9664,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="212" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="7">
         <v>43620.486011516201</v>
       </c>
@@ -9705,7 +9705,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="213" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="7">
         <v>43620.487928645831</v>
       </c>
@@ -9734,7 +9734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="7">
         <v>43620.488378425929</v>
       </c>
@@ -9754,7 +9754,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="215" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="7">
         <v>43620.488762453708</v>
       </c>
@@ -9774,7 +9774,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="216" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="7">
         <v>43620.502757766204</v>
       </c>
@@ -9803,7 +9803,7 @@
         <v>8700</v>
       </c>
     </row>
-    <row r="217" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="7">
         <v>43620.503008993051</v>
       </c>
@@ -9844,7 +9844,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="218" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="7">
         <v>43620.516394976847</v>
       </c>
@@ -9870,7 +9870,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="219" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="7">
         <v>43620.531383842594</v>
       </c>
@@ -9893,7 +9893,7 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="220" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="7">
         <v>43620.534318229169</v>
       </c>
@@ -9922,7 +9922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="7">
         <v>43620.53862825231</v>
       </c>
@@ -9951,7 +9951,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="222" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="7">
         <v>43620.544621446759</v>
       </c>
@@ -9980,7 +9980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="7">
         <v>43620.559045000002</v>
       </c>
@@ -10021,7 +10021,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="224" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="7">
         <v>43620.562107916667</v>
       </c>
@@ -10044,7 +10044,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="225" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="7">
         <v>43620.57524528935</v>
       </c>
@@ -10085,7 +10085,7 @@
         <v>1540</v>
       </c>
     </row>
-    <row r="226" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="7">
         <v>43620.57848960648</v>
       </c>
@@ -10114,7 +10114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="7">
         <v>43620.589187465273</v>
       </c>
@@ -10137,7 +10137,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="228" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="7">
         <v>43620.646162557867</v>
       </c>
@@ -10178,7 +10178,7 @@
         <v>2215</v>
       </c>
     </row>
-    <row r="229" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="7">
         <v>43620.686772013883</v>
       </c>
@@ -10201,7 +10201,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="230" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="7">
         <v>43623.521720659723</v>
       </c>
@@ -10224,7 +10224,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="231" spans="1:15" s="22" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:15" s="22" customFormat="1" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="18">
         <v>43623.522309618056</v>
       </c>
@@ -10247,7 +10247,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="232" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="7">
         <v>43633.40398304398</v>
       </c>
@@ -10276,7 +10276,7 @@
         <v>5100</v>
       </c>
     </row>
-    <row r="233" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="7">
         <v>43633.416756932871</v>
       </c>
@@ -10305,7 +10305,7 @@
         <v>5100</v>
       </c>
     </row>
-    <row r="234" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="7">
         <v>43633.420208194446</v>
       </c>
@@ -10334,7 +10334,7 @@
         <v>14250</v>
       </c>
     </row>
-    <row r="235" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="7">
         <v>43633.428534791667</v>
       </c>
@@ -10363,7 +10363,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="236" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="7">
         <v>43633.4461915625</v>
       </c>
@@ -10392,7 +10392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="7">
         <v>43633.46175555556</v>
       </c>
@@ -10436,7 +10436,7 @@
         <v>2270</v>
       </c>
     </row>
-    <row r="238" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="7">
         <v>43633.50244113426</v>
       </c>
@@ -10465,7 +10465,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="239" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="7">
         <v>43633.504802060183</v>
       </c>
@@ -10494,7 +10494,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="240" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="7">
         <v>43633.523931469907</v>
       </c>
@@ -10523,7 +10523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" s="7">
         <v>43633.530496736115</v>
       </c>
@@ -10567,7 +10567,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="242" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="7">
         <v>43633.533061898153</v>
       </c>
@@ -10596,7 +10596,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="243" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="7">
         <v>43633.539491469906</v>
       </c>
@@ -10625,7 +10625,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="244" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="7">
         <v>43633.543584953703</v>
       </c>
@@ -10654,7 +10654,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="245" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" s="7">
         <v>43633.547313564814</v>
       </c>
@@ -10683,7 +10683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="7">
         <v>43633.551025127315</v>
       </c>
@@ -10712,7 +10712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="7">
         <v>43633.562344479171</v>
       </c>
@@ -10785,7 +10785,7 @@
         <v>9400</v>
       </c>
     </row>
-    <row r="249" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="7">
         <v>43633.581785532406</v>
       </c>
@@ -10869,7 +10869,7 @@
         <v>7400</v>
       </c>
     </row>
-    <row r="252" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="7">
         <v>43633.63865868056</v>
       </c>
@@ -10901,7 +10901,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="253" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" s="7">
         <v>43633.660197569443</v>
       </c>
@@ -10933,7 +10933,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="254" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" s="7">
         <v>43633.689922777776</v>
       </c>
@@ -10965,7 +10965,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="255" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" s="7">
         <v>43634.393672152779</v>
       </c>
@@ -10994,7 +10994,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="256" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" s="7">
         <v>43634.396875138889</v>
       </c>
@@ -11023,7 +11023,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="257" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" s="7">
         <v>43634.405545023154</v>
       </c>
@@ -11052,7 +11052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" s="7">
         <v>43634.416232280091</v>
       </c>
@@ -11081,7 +11081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" s="7">
         <v>43634.420364861115</v>
       </c>
@@ -11110,7 +11110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" s="7">
         <v>43634.424504351853</v>
       </c>
@@ -11154,7 +11154,7 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="261" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" s="7">
         <v>43634.427363206021</v>
       </c>
@@ -11183,7 +11183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" s="7">
         <v>43634.437920937504</v>
       </c>
@@ -11212,7 +11212,7 @@
         <v>7250</v>
       </c>
     </row>
-    <row r="263" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" s="7">
         <v>43634.446620960647</v>
       </c>
@@ -11241,7 +11241,7 @@
         <v>9500</v>
       </c>
     </row>
-    <row r="264" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" s="7">
         <v>43634.454626250001</v>
       </c>
@@ -11270,7 +11270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" s="7">
         <v>43634.456643518519</v>
       </c>
@@ -11302,7 +11302,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="266" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" s="7">
         <v>43634.458449259255</v>
       </c>
@@ -11331,7 +11331,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="267" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" s="7">
         <v>43634.469420011577</v>
       </c>
@@ -11360,7 +11360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" s="7">
         <v>43634.472232048611</v>
       </c>
@@ -11389,7 +11389,7 @@
         <v>3400</v>
       </c>
     </row>
-    <row r="269" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" s="7">
         <v>43634.478026145836</v>
       </c>
@@ -11418,7 +11418,7 @@
         <v>3150</v>
       </c>
     </row>
-    <row r="270" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" s="7">
         <v>43634.478377719905</v>
       </c>
@@ -11447,7 +11447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" s="7">
         <v>43634.486881469908</v>
       </c>
@@ -11476,7 +11476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" s="7">
         <v>43634.488325983795</v>
       </c>
@@ -11505,7 +11505,7 @@
         <v>8100</v>
       </c>
     </row>
-    <row r="273" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" s="7">
         <v>43634.496477800931</v>
       </c>
@@ -11537,7 +11537,7 @@
         <v>8100</v>
       </c>
     </row>
-    <row r="274" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" s="7">
         <v>43634.500037627316</v>
       </c>
@@ -11566,7 +11566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" s="7">
         <v>43634.503317557872</v>
       </c>
@@ -11595,7 +11595,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="276" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" s="7">
         <v>43634.5105887963</v>
       </c>
@@ -11624,7 +11624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" s="7">
         <v>43634.51392675926</v>
       </c>
@@ -11656,7 +11656,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="278" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" s="7">
         <v>43634.530469999998</v>
       </c>
@@ -11685,7 +11685,7 @@
         <v>1760</v>
       </c>
     </row>
-    <row r="279" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" s="7">
         <v>43634.56578636574</v>
       </c>
@@ -11717,7 +11717,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="280" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" s="7">
         <v>43634.579063877318</v>
       </c>
@@ -11743,7 +11743,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="281" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" s="7">
         <v>43634.582968854171</v>
       </c>
@@ -11775,7 +11775,7 @@
         <v>1420</v>
       </c>
     </row>
-    <row r="282" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" s="7">
         <v>43634.633482164354</v>
       </c>
@@ -11804,7 +11804,7 @@
         <v>5100</v>
       </c>
     </row>
-    <row r="283" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" s="7">
         <v>43637.422400451389</v>
       </c>
@@ -11833,7 +11833,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="284" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" s="7">
         <v>43641.40604130787</v>
       </c>
@@ -11874,7 +11874,7 @@
         <v>3015</v>
       </c>
     </row>
-    <row r="285" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" s="7">
         <v>43641.415160428238</v>
       </c>
@@ -11915,7 +11915,7 @@
         <v>2750</v>
       </c>
     </row>
-    <row r="286" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" s="7">
         <v>43641.438067060182</v>
       </c>
@@ -11956,7 +11956,7 @@
         <v>2620</v>
       </c>
     </row>
-    <row r="287" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" s="7">
         <v>43641.454948587962</v>
       </c>
@@ -11997,7 +11997,7 @@
         <v>2475</v>
       </c>
     </row>
-    <row r="288" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" s="7">
         <v>43641.468790266204</v>
       </c>
@@ -12079,7 +12079,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="290" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" s="7">
         <v>43641.555053761578</v>
       </c>
@@ -12120,7 +12120,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="291" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" s="7">
         <v>43641.635631805555</v>
       </c>
@@ -12161,7 +12161,7 @@
         <v>1815</v>
       </c>
     </row>
-    <row r="292" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" s="7">
         <v>43641.647440000001</v>
       </c>
@@ -12202,7 +12202,7 @@
         <v>1565</v>
       </c>
     </row>
-    <row r="293" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" s="7">
         <v>43641.6602040625</v>
       </c>
@@ -12243,7 +12243,7 @@
         <v>1645</v>
       </c>
     </row>
-    <row r="294" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" s="7">
         <v>43641.689663888887</v>
       </c>
@@ -12284,7 +12284,7 @@
         <v>1730</v>
       </c>
     </row>
-    <row r="295" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" s="7">
         <v>43641.701291400459</v>
       </c>
@@ -12325,7 +12325,7 @@
         <v>1930</v>
       </c>
     </row>
-    <row r="296" spans="1:17" s="22" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:17" s="22" customFormat="1" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" s="18">
         <v>43641.717524178239</v>
       </c>
@@ -12369,7 +12369,7 @@
         <v>2120</v>
       </c>
     </row>
-    <row r="297" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" s="7">
         <v>43647.378567395834</v>
       </c>
@@ -12402,7 +12402,7 @@
       </c>
       <c r="Q297" s="5"/>
     </row>
-    <row r="298" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" s="7">
         <v>43647.39412060185</v>
       </c>
@@ -12435,7 +12435,7 @@
       </c>
       <c r="Q298" s="5"/>
     </row>
-    <row r="299" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" s="7">
         <v>43647.403549803239</v>
       </c>
@@ -12468,7 +12468,7 @@
       </c>
       <c r="Q299" s="5"/>
     </row>
-    <row r="300" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" s="7">
         <v>43647.418112916668</v>
       </c>
@@ -12501,7 +12501,7 @@
       </c>
       <c r="Q300" s="5"/>
     </row>
-    <row r="301" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" s="7">
         <v>43647.437997430556</v>
       </c>
@@ -12533,7 +12533,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="302" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" s="7">
         <v>43647.442859641204</v>
       </c>
@@ -12566,7 +12566,7 @@
       </c>
       <c r="Q302" s="5"/>
     </row>
-    <row r="303" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" s="7">
         <v>43647.44526699074</v>
       </c>
@@ -12599,7 +12599,7 @@
       </c>
       <c r="Q303" s="5"/>
     </row>
-    <row r="304" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" s="7">
         <v>43647.445862928245</v>
       </c>
@@ -12632,7 +12632,7 @@
       </c>
       <c r="Q304" s="5"/>
     </row>
-    <row r="305" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" s="7">
         <v>43647.452365173609</v>
       </c>
@@ -12665,7 +12665,7 @@
       </c>
       <c r="Q305" s="5"/>
     </row>
-    <row r="306" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" s="7">
         <v>43647.46204752315</v>
       </c>
@@ -12698,7 +12698,7 @@
       </c>
       <c r="Q306" s="5"/>
     </row>
-    <row r="307" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" s="7">
         <v>43647.47148359954</v>
       </c>
@@ -12731,7 +12731,7 @@
       </c>
       <c r="Q307" s="5"/>
     </row>
-    <row r="308" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" s="7">
         <v>43647.475172638893</v>
       </c>
@@ -12764,7 +12764,7 @@
       </c>
       <c r="Q308" s="5"/>
     </row>
-    <row r="309" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" s="7">
         <v>43647.482570231485</v>
       </c>
@@ -12797,7 +12797,7 @@
       </c>
       <c r="Q309" s="5"/>
     </row>
-    <row r="310" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" s="7">
         <v>43647.489491956017</v>
       </c>
@@ -12863,7 +12863,7 @@
       </c>
       <c r="Q311" s="5"/>
     </row>
-    <row r="312" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" s="7">
         <v>43647.496494571758</v>
       </c>
@@ -12896,7 +12896,7 @@
       </c>
       <c r="Q312" s="5"/>
     </row>
-    <row r="313" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" s="7">
         <v>43647.5053858912</v>
       </c>
@@ -12965,7 +12965,7 @@
       </c>
       <c r="Q314" s="5"/>
     </row>
-    <row r="315" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" s="7">
         <v>43647.513685578699</v>
       </c>
@@ -13067,7 +13067,7 @@
       </c>
       <c r="Q317" s="5"/>
     </row>
-    <row r="318" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" s="7">
         <v>43647.535344895834</v>
       </c>
@@ -13100,7 +13100,7 @@
       </c>
       <c r="Q318" s="5"/>
     </row>
-    <row r="319" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" s="7">
         <v>43647.537166388887</v>
       </c>
@@ -13133,7 +13133,7 @@
       </c>
       <c r="Q319" s="5"/>
     </row>
-    <row r="320" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320" s="7">
         <v>43647.538050277777</v>
       </c>
@@ -13166,7 +13166,7 @@
       </c>
       <c r="Q320" s="5"/>
     </row>
-    <row r="321" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" s="7">
         <v>43647.540616631944</v>
       </c>
@@ -13199,7 +13199,7 @@
       </c>
       <c r="Q321" s="5"/>
     </row>
-    <row r="322" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" s="7">
         <v>43647.54435773148</v>
       </c>
@@ -13232,7 +13232,7 @@
       </c>
       <c r="Q322" s="5"/>
     </row>
-    <row r="323" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" s="7">
         <v>43647.547887106484</v>
       </c>
@@ -13265,7 +13265,7 @@
       </c>
       <c r="Q323" s="5"/>
     </row>
-    <row r="324" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" s="7">
         <v>43647.551679976852</v>
       </c>
@@ -13298,7 +13298,7 @@
       </c>
       <c r="Q324" s="5"/>
     </row>
-    <row r="325" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" s="7">
         <v>43647.55485487268</v>
       </c>
@@ -13331,7 +13331,7 @@
       </c>
       <c r="Q325" s="5"/>
     </row>
-    <row r="326" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" s="7">
         <v>43647.586594768523</v>
       </c>
@@ -13367,7 +13367,7 @@
       </c>
       <c r="Q326" s="5"/>
     </row>
-    <row r="327" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" s="7">
         <v>43647.578063356486</v>
       </c>
@@ -13400,7 +13400,7 @@
       </c>
       <c r="Q327" s="5"/>
     </row>
-    <row r="328" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" s="7">
         <v>43647.581616527779</v>
       </c>
@@ -13436,7 +13436,7 @@
       </c>
       <c r="Q328" s="5"/>
     </row>
-    <row r="329" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" s="7">
         <v>43647.586999560182</v>
       </c>
@@ -13472,7 +13472,7 @@
       </c>
       <c r="Q329" s="5"/>
     </row>
-    <row r="330" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" s="7">
         <v>43647.587708356485</v>
       </c>
@@ -13505,7 +13505,7 @@
       </c>
       <c r="Q330" s="5"/>
     </row>
-    <row r="331" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" s="7">
         <v>43647.58930334491</v>
       </c>
@@ -13538,7 +13538,7 @@
       </c>
       <c r="Q331" s="5"/>
     </row>
-    <row r="332" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" s="7">
         <v>43647.614860520829</v>
       </c>
@@ -13571,7 +13571,7 @@
       </c>
       <c r="Q332" s="5"/>
     </row>
-    <row r="333" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333" s="7">
         <v>43647.616616493055</v>
       </c>
@@ -13604,7 +13604,7 @@
       </c>
       <c r="Q333" s="5"/>
     </row>
-    <row r="334" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334" s="7">
         <v>43647.628458217594</v>
       </c>
@@ -13631,7 +13631,7 @@
       </c>
       <c r="Q334" s="5"/>
     </row>
-    <row r="335" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335" s="7">
         <v>43647.648176006944</v>
       </c>
@@ -13664,7 +13664,7 @@
       </c>
       <c r="Q335" s="5"/>
     </row>
-    <row r="336" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" s="7">
         <v>43647.652004189818</v>
       </c>
@@ -13697,7 +13697,7 @@
       </c>
       <c r="Q336" s="5"/>
     </row>
-    <row r="337" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" s="7">
         <v>43647.663755868052</v>
       </c>
@@ -13730,7 +13730,7 @@
       </c>
       <c r="Q337" s="5"/>
     </row>
-    <row r="338" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" s="7">
         <v>43648.434577314816</v>
       </c>
@@ -13766,7 +13766,7 @@
       </c>
       <c r="Q338" s="5"/>
     </row>
-    <row r="339" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339" s="7">
         <v>43648.464827615739</v>
       </c>
@@ -13799,7 +13799,7 @@
       </c>
       <c r="Q339" s="5"/>
     </row>
-    <row r="340" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340" s="7">
         <v>43648.49087303241</v>
       </c>
@@ -13829,7 +13829,7 @@
       </c>
       <c r="Q340" s="5"/>
     </row>
-    <row r="341" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341" s="7">
         <v>43648.505817361111</v>
       </c>
@@ -13862,7 +13862,7 @@
       </c>
       <c r="Q341" s="5"/>
     </row>
-    <row r="342" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342" s="7">
         <v>43648.523454918977</v>
       </c>
@@ -13892,7 +13892,7 @@
       </c>
       <c r="Q342" s="5"/>
     </row>
-    <row r="343" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343" s="7">
         <v>43648.535805590276</v>
       </c>
@@ -13918,7 +13918,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="344" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" s="7">
         <v>43648.557352407406</v>
       </c>
@@ -13951,7 +13951,7 @@
       </c>
       <c r="Q344" s="5"/>
     </row>
-    <row r="345" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345" s="7">
         <v>43648.574154016205</v>
       </c>
@@ -13987,7 +13987,7 @@
       </c>
       <c r="Q345" s="5"/>
     </row>
-    <row r="346" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" s="7">
         <v>43648.597286747681</v>
       </c>
@@ -14020,7 +14020,7 @@
       </c>
       <c r="Q346" s="5"/>
     </row>
-    <row r="347" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347" s="7">
         <v>43648.600304039355</v>
       </c>
@@ -14053,7 +14053,7 @@
       </c>
       <c r="Q347" s="5"/>
     </row>
-    <row r="348" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" s="7">
         <v>43648.61853983796</v>
       </c>
@@ -14089,7 +14089,7 @@
       </c>
       <c r="Q348" s="5"/>
     </row>
-    <row r="349" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" s="7">
         <v>43657.492113460648</v>
       </c>
@@ -14118,7 +14118,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="350" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350" s="7">
         <v>43657.493938182874</v>
       </c>
@@ -14150,7 +14150,7 @@
         <v>1597</v>
       </c>
     </row>
-    <row r="351" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A351" s="25">
         <v>43661.402646550923</v>
       </c>
@@ -14182,7 +14182,7 @@
         <v>2190</v>
       </c>
     </row>
-    <row r="352" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A352" s="25">
         <v>43661.407537430554</v>
       </c>
@@ -14214,7 +14214,7 @@
         <v>32.43</v>
       </c>
     </row>
-    <row r="353" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A353" s="25">
         <v>43661.419768958338</v>
       </c>
@@ -14246,7 +14246,7 @@
         <v>2066</v>
       </c>
     </row>
-    <row r="354" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A354" s="25">
         <v>43661.427344340278</v>
       </c>
@@ -14278,7 +14278,7 @@
         <v>2407</v>
       </c>
     </row>
-    <row r="355" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A355" s="25">
         <v>43661.429183032407</v>
       </c>
@@ -14307,7 +14307,7 @@
         <v>2280</v>
       </c>
     </row>
-    <row r="356" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A356" s="25">
         <v>43661.441045312502</v>
       </c>
@@ -14339,7 +14339,7 @@
         <v>5957</v>
       </c>
     </row>
-    <row r="357" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A357" s="25">
         <v>43661.454036006944</v>
       </c>
@@ -14371,7 +14371,7 @@
         <v>1830</v>
       </c>
     </row>
-    <row r="358" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A358" s="25">
         <v>43661.463808819448</v>
       </c>
@@ -14403,7 +14403,7 @@
         <v>5707</v>
       </c>
     </row>
-    <row r="359" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A359" s="25">
         <v>43661.465437303239</v>
       </c>
@@ -14435,7 +14435,7 @@
         <v>2455</v>
       </c>
     </row>
-    <row r="360" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A360" s="25">
         <v>43661.470525659723</v>
       </c>
@@ -14464,7 +14464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="361" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A361" s="25">
         <v>43661.475225057875</v>
       </c>
@@ -14496,7 +14496,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="362" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A362" s="25">
         <v>43661.488394363427</v>
       </c>
@@ -14528,7 +14528,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="363" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A363" s="25">
         <v>43661.49257905093</v>
       </c>
@@ -14560,7 +14560,7 @@
         <v>1940</v>
       </c>
     </row>
-    <row r="364" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A364" s="25">
         <v>43661.496228148149</v>
       </c>
@@ -14592,7 +14592,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="365" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A365" s="25">
         <v>43661.502193263892</v>
       </c>
@@ -14624,7 +14624,7 @@
         <v>3342</v>
       </c>
     </row>
-    <row r="366" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A366" s="25">
         <v>43661.52084143518</v>
       </c>
@@ -14656,7 +14656,7 @@
         <v>1672</v>
       </c>
     </row>
-    <row r="367" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A367" s="25">
         <v>43661.539627453705</v>
       </c>
@@ -14688,7 +14688,7 @@
         <v>1442</v>
       </c>
     </row>
-    <row r="368" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A368" s="25">
         <v>43661.544727465276</v>
       </c>
@@ -14778,7 +14778,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="371" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A371" s="25">
         <v>43661.595967152782</v>
       </c>
@@ -14807,7 +14807,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="372" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A372" s="25">
         <v>43662.505582557875</v>
       </c>
@@ -14839,7 +14839,7 @@
         <v>4650</v>
       </c>
     </row>
-    <row r="373" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A373" s="25">
         <v>43662.403231944445</v>
       </c>
@@ -14871,7 +14871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="374" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A374" s="25">
         <v>43662.417311712961</v>
       </c>
@@ -14903,7 +14903,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="375" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A375" s="25">
         <v>43662.423942743058</v>
       </c>
@@ -14935,7 +14935,7 @@
         <v>3077</v>
       </c>
     </row>
-    <row r="376" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A376" s="25">
         <v>43662.43173575231</v>
       </c>
@@ -14964,7 +14964,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="377" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A377" s="25">
         <v>43662.438895104162</v>
       </c>
@@ -14993,7 +14993,7 @@
         <v>2620</v>
       </c>
     </row>
-    <row r="378" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A378" s="25">
         <v>43662.457425300927</v>
       </c>
@@ -15022,7 +15022,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="379" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A379" s="25">
         <v>43662.470728321758</v>
       </c>
@@ -15054,7 +15054,7 @@
         <v>1778</v>
       </c>
     </row>
-    <row r="380" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A380" s="25">
         <v>43662.481005601847</v>
       </c>
@@ -15086,7 +15086,7 @@
         <v>1844</v>
       </c>
     </row>
-    <row r="381" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A381" s="25">
         <v>43662.503588680556</v>
       </c>
@@ -15118,7 +15118,7 @@
         <v>1834</v>
       </c>
     </row>
-    <row r="382" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A382" s="25">
         <v>43662.508576585649</v>
       </c>
@@ -15150,7 +15150,7 @@
         <v>2690</v>
       </c>
     </row>
-    <row r="383" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A383" s="25">
         <v>43662.515664699073</v>
       </c>
@@ -15182,7 +15182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="384" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A384" s="25">
         <v>43662.523681469909</v>
       </c>
@@ -15214,7 +15214,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="385" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A385" s="25">
         <v>43662.524749976852</v>
       </c>
@@ -15246,7 +15246,7 @@
         <v>2651</v>
       </c>
     </row>
-    <row r="386" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A386" s="25">
         <v>43662.526702222225</v>
       </c>
@@ -15278,7 +15278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="387" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A387" s="25">
         <v>43662.528149259262</v>
       </c>
@@ -15308,7 +15308,7 @@
         <v>999999999</v>
       </c>
     </row>
-    <row r="388" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A388" s="25">
         <v>43662.530195763888</v>
       </c>
@@ -15340,7 +15340,7 @@
         <v>2690</v>
       </c>
     </row>
-    <row r="389" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A389" s="25">
         <v>43662.533871203705</v>
       </c>
@@ -15372,7 +15372,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="390" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A390" s="25">
         <v>43662.534038217593</v>
       </c>
@@ -15404,7 +15404,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="391" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A391" s="25">
         <v>43662.552655601852</v>
       </c>
@@ -15436,7 +15436,7 @@
         <v>1820</v>
       </c>
     </row>
-    <row r="392" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A392" s="25">
         <v>43662.553831041667</v>
       </c>
@@ -15468,7 +15468,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="393" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A393" s="25">
         <v>43662.553892222219</v>
       </c>
@@ -15497,7 +15497,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="394" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A394" s="25">
         <v>43662.576265393523</v>
       </c>
@@ -15526,7 +15526,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="395" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A395" s="25">
         <v>43662.605140277781</v>
       </c>
@@ -15558,7 +15558,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="396" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A396" s="25">
         <v>43662.608947546294</v>
       </c>
@@ -15587,7 +15587,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="397" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A397" s="25">
         <v>43662.630076076384</v>
       </c>
@@ -15610,7 +15610,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="398" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A398" s="25">
         <v>43662.638398935189</v>
       </c>
@@ -15639,7 +15639,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="399" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A399" s="25">
         <v>43662.651400266201</v>
       </c>
@@ -15668,7 +15668,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="400" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A400" s="25">
         <v>43662.653115231486</v>
       </c>
@@ -15697,7 +15697,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="401" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:23" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A401" s="25">
         <v>43662.868660763888</v>
       </c>
@@ -15755,7 +15755,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="403" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A403" s="25">
         <v>43665.538775069443</v>
       </c>
@@ -15778,7 +15778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="404" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:23" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A404" s="25">
         <v>43665.565719756945</v>
       </c>
@@ -15807,7 +15807,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="405" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:23" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A405" s="25">
         <v>43665.602270196759</v>
       </c>
@@ -15836,7 +15836,7 @@
         <v>1420</v>
       </c>
     </row>
-    <row r="406" spans="1:23" s="34" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:23" s="34" customFormat="1" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A406" s="30">
         <v>43665.620232199071</v>
       </c>
@@ -15865,7 +15865,7 @@
         <v>2590</v>
       </c>
     </row>
-    <row r="407" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A407" s="35">
         <v>43676.683530092596</v>
       </c>
@@ -15912,7 +15912,7 @@
       <c r="V407" s="36"/>
       <c r="W407" s="36"/>
     </row>
-    <row r="408" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A408" s="35">
         <v>43677.336412037039</v>
       </c>
@@ -15955,7 +15955,7 @@
       <c r="V408" s="36"/>
       <c r="W408" s="36"/>
     </row>
-    <row r="409" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A409" s="35">
         <v>43677.349629629629</v>
       </c>
@@ -15998,7 +15998,7 @@
       <c r="V409" s="36"/>
       <c r="W409" s="36"/>
     </row>
-    <row r="410" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A410" s="35">
         <v>43677.356956018521</v>
       </c>
@@ -16041,7 +16041,7 @@
       <c r="V410" s="36"/>
       <c r="W410" s="36"/>
     </row>
-    <row r="411" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A411" s="35">
         <v>43677.370138888888</v>
       </c>
@@ -16084,7 +16084,7 @@
       <c r="V411" s="36"/>
       <c r="W411" s="36"/>
     </row>
-    <row r="412" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A412" s="35">
         <v>43677.411805555559</v>
       </c>
@@ -16123,7 +16123,7 @@
       <c r="V412" s="36"/>
       <c r="W412" s="36"/>
     </row>
-    <row r="413" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A413" s="35">
         <v>43677.412245370368</v>
       </c>
@@ -16248,7 +16248,7 @@
       <c r="V415" s="36"/>
       <c r="W415" s="36"/>
     </row>
-    <row r="416" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A416" s="35">
         <v>43677.419004629628</v>
       </c>
@@ -16293,7 +16293,7 @@
       <c r="V416" s="36"/>
       <c r="W416" s="36"/>
     </row>
-    <row r="417" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A417" s="35">
         <v>43677.428067129629</v>
       </c>
@@ -16338,7 +16338,7 @@
       <c r="V417" s="36"/>
       <c r="W417" s="36"/>
     </row>
-    <row r="418" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A418" s="35">
         <v>43677.428483796299</v>
       </c>
@@ -16383,7 +16383,7 @@
       <c r="V418" s="36"/>
       <c r="W418" s="36"/>
     </row>
-    <row r="419" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A419" s="35">
         <v>43677.430266203701</v>
       </c>
@@ -16426,7 +16426,7 @@
       <c r="V419" s="36"/>
       <c r="W419" s="36"/>
     </row>
-    <row r="420" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A420" s="35">
         <v>43677.437337962961</v>
       </c>
@@ -16471,7 +16471,7 @@
       <c r="V420" s="36"/>
       <c r="W420" s="36"/>
     </row>
-    <row r="421" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A421" s="35">
         <v>43677.448240740741</v>
       </c>
@@ -16516,7 +16516,7 @@
       <c r="V421" s="36"/>
       <c r="W421" s="36"/>
     </row>
-    <row r="422" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A422" s="35">
         <v>43677.465532407405</v>
       </c>
@@ -16561,7 +16561,7 @@
       <c r="V422" s="36"/>
       <c r="W422" s="36"/>
     </row>
-    <row r="423" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A423" s="35">
         <v>43677.49422453704</v>
       </c>
@@ -16600,7 +16600,7 @@
       <c r="V423" s="36"/>
       <c r="W423" s="36"/>
     </row>
-    <row r="424" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A424" s="35">
         <v>43677.491331018522</v>
       </c>
@@ -16645,7 +16645,7 @@
       <c r="V424" s="36"/>
       <c r="W424" s="36"/>
     </row>
-    <row r="425" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A425" s="35">
         <v>43677.509918981479</v>
       </c>
@@ -16690,7 +16690,7 @@
       <c r="V425" s="36"/>
       <c r="W425" s="36"/>
     </row>
-    <row r="426" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A426" s="35">
         <v>43677.511956018519</v>
       </c>
@@ -16735,7 +16735,7 @@
       <c r="V426" s="36"/>
       <c r="W426" s="36"/>
     </row>
-    <row r="427" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A427" s="35">
         <v>43677.514525462961</v>
       </c>
@@ -16774,7 +16774,7 @@
       <c r="V427" s="36"/>
       <c r="W427" s="36"/>
     </row>
-    <row r="428" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A428" s="35">
         <v>43677.518958333334</v>
       </c>
@@ -16819,7 +16819,7 @@
       <c r="V428" s="36"/>
       <c r="W428" s="36"/>
     </row>
-    <row r="429" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A429" s="35">
         <v>43677.520370370374</v>
       </c>
@@ -16864,7 +16864,7 @@
       <c r="V429" s="36"/>
       <c r="W429" s="36"/>
     </row>
-    <row r="430" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A430" s="35">
         <v>43677.52925925926</v>
       </c>
@@ -16909,7 +16909,7 @@
       <c r="V430" s="36"/>
       <c r="W430" s="36"/>
     </row>
-    <row r="431" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A431" s="35">
         <v>43677.537638888891</v>
       </c>
@@ -16954,7 +16954,7 @@
       <c r="V431" s="36"/>
       <c r="W431" s="36"/>
     </row>
-    <row r="432" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A432" s="35">
         <v>43677.549780092595</v>
       </c>
@@ -16997,7 +16997,7 @@
       <c r="V432" s="36"/>
       <c r="W432" s="36"/>
     </row>
-    <row r="433" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A433" s="35">
         <v>43677.553333333337</v>
       </c>
@@ -17042,7 +17042,7 @@
       <c r="V433" s="36"/>
       <c r="W433" s="36"/>
     </row>
-    <row r="434" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A434" s="35">
         <v>43677.671620370369</v>
       </c>
@@ -17085,7 +17085,7 @@
       <c r="V434" s="36"/>
       <c r="W434" s="36"/>
     </row>
-    <row r="435" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A435" s="35">
         <v>43678.3440162037</v>
       </c>
@@ -17128,7 +17128,7 @@
       <c r="V435" s="36"/>
       <c r="W435" s="36"/>
     </row>
-    <row r="436" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A436" s="35">
         <v>43678.348865740743</v>
       </c>
@@ -17171,7 +17171,7 @@
       <c r="V436" s="36"/>
       <c r="W436" s="36"/>
     </row>
-    <row r="437" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A437" s="35">
         <v>43678.354548611111</v>
       </c>
@@ -17214,7 +17214,7 @@
       <c r="V437" s="36"/>
       <c r="W437" s="36"/>
     </row>
-    <row r="438" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A438" s="35">
         <v>43678.363217592596</v>
       </c>
@@ -17257,7 +17257,7 @@
       <c r="V438" s="36"/>
       <c r="W438" s="36"/>
     </row>
-    <row r="439" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A439" s="35">
         <v>43678.372650462959</v>
       </c>
@@ -17300,7 +17300,7 @@
       <c r="V439" s="36"/>
       <c r="W439" s="36"/>
     </row>
-    <row r="440" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A440" s="35">
         <v>43678.375023148146</v>
       </c>
@@ -17343,7 +17343,7 @@
       <c r="V440" s="36"/>
       <c r="W440" s="36"/>
     </row>
-    <row r="441" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A441" s="35">
         <v>43678.389131944445</v>
       </c>
@@ -17386,7 +17386,7 @@
       <c r="V441" s="36"/>
       <c r="W441" s="36"/>
     </row>
-    <row r="442" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A442" s="35">
         <v>43678.390729166669</v>
       </c>
@@ -17429,7 +17429,7 @@
       <c r="V442" s="36"/>
       <c r="W442" s="36"/>
     </row>
-    <row r="443" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A443" s="35">
         <v>43678.404270833336</v>
       </c>
@@ -17472,7 +17472,7 @@
       <c r="V443" s="36"/>
       <c r="W443" s="36"/>
     </row>
-    <row r="444" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A444" s="35">
         <v>43678.408738425926</v>
       </c>
@@ -17517,7 +17517,7 @@
       <c r="V444" s="36"/>
       <c r="W444" s="36"/>
     </row>
-    <row r="445" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A445" s="35">
         <v>43678.415671296294</v>
       </c>
@@ -17562,7 +17562,7 @@
       <c r="V445" s="36"/>
       <c r="W445" s="36"/>
     </row>
-    <row r="446" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A446" s="35">
         <v>43678.425798611112</v>
       </c>
@@ -17607,7 +17607,7 @@
       <c r="V446" s="36"/>
       <c r="W446" s="36"/>
     </row>
-    <row r="447" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A447" s="35">
         <v>43678.438703703701</v>
       </c>
@@ -17652,7 +17652,7 @@
       <c r="V447" s="36"/>
       <c r="W447" s="36"/>
     </row>
-    <row r="448" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A448" s="35">
         <v>43678.447800925926</v>
       </c>
@@ -17697,7 +17697,7 @@
       <c r="V448" s="36"/>
       <c r="W448" s="36"/>
     </row>
-    <row r="449" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A449" s="35">
         <v>43678.504062499997</v>
       </c>
@@ -17742,7 +17742,7 @@
       <c r="V449" s="36"/>
       <c r="W449" s="36"/>
     </row>
-    <row r="450" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A450" s="35">
         <v>43678.518854166665</v>
       </c>
@@ -17787,7 +17787,7 @@
       <c r="V450" s="36"/>
       <c r="W450" s="36"/>
     </row>
-    <row r="451" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A451" s="35">
         <v>43678.522696759261</v>
       </c>
@@ -17832,7 +17832,7 @@
       <c r="V451" s="36"/>
       <c r="W451" s="36"/>
     </row>
-    <row r="452" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A452" s="35">
         <v>43678.557997685188</v>
       </c>
@@ -17877,7 +17877,7 @@
       <c r="V452" s="36"/>
       <c r="W452" s="36"/>
     </row>
-    <row r="453" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A453" s="35">
         <v>43678.558668981481</v>
       </c>
@@ -17922,7 +17922,7 @@
       <c r="V453" s="36"/>
       <c r="W453" s="36"/>
     </row>
-    <row r="454" spans="1:23" s="34" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:23" s="34" customFormat="1" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A454" s="42">
         <v>43678.562905092593</v>
       </c>
@@ -17968,7 +17968,14 @@
       <c r="W454" s="43"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U350"/>
+  <autoFilter ref="A1:U454">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="SLR-045A"/>
+        <filter val="SLR-045B"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1"/>
     <hyperlink ref="G6" r:id="rId2"/>

</xml_diff>

<commit_message>
I got all the SLR and SWT done
</commit_message>
<xml_diff>
--- a/0 - Field Data Sheets/Weir Calibration Field Form 2019 CURRENT 07_31_2019.xlsx
+++ b/0 - Field Data Sheets/Weir Calibration Field Form 2019 CURRENT 07_31_2019.xlsx
@@ -1961,7 +1961,7 @@
         <xdr:cNvPr id="2" name="EsriDoNotEdit">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2309,9 +2309,9 @@
   </sheetPr>
   <dimension ref="A1:W454"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K416" sqref="K416"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A194" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B218" sqref="B218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2600,7 +2600,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>43591.472597476852</v>
       </c>
@@ -4190,7 +4190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
         <v>43593.619830208336</v>
       </c>
@@ -4231,7 +4231,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7">
         <v>43593.656584456017</v>
       </c>
@@ -6520,7 +6520,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="119" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="7">
         <v>43595.569374467595</v>
       </c>
@@ -8881,7 +8881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A185" s="7">
         <v>43619.417066539347</v>
       </c>
@@ -8910,7 +8910,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="186" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A186" s="7">
         <v>43619.424325891203</v>
       </c>
@@ -8945,7 +8945,7 @@
         <v>8600</v>
       </c>
     </row>
-    <row r="187" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A187" s="7">
         <v>43619.430370590278</v>
       </c>
@@ -8974,7 +8974,7 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="188" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A188" s="7">
         <v>43619.448148344905</v>
       </c>
@@ -8997,7 +8997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A189" s="7">
         <v>43619.449386782406</v>
       </c>
@@ -9041,7 +9041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A190" s="7">
         <v>43619.457925891205</v>
       </c>
@@ -9085,7 +9085,7 @@
         <v>4910</v>
       </c>
     </row>
-    <row r="191" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A191" s="7">
         <v>43619.481042361112</v>
       </c>
@@ -9114,7 +9114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A192" s="7">
         <v>43619.482240219906</v>
       </c>
@@ -9143,7 +9143,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="193" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A193" s="7">
         <v>43619.485708449072</v>
       </c>
@@ -9172,7 +9172,7 @@
         <v>2470</v>
       </c>
     </row>
-    <row r="194" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A194" s="7">
         <v>43619.502512523148</v>
       </c>
@@ -9201,7 +9201,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="195" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A195" s="7">
         <v>43619.50333712963</v>
       </c>
@@ -9224,7 +9224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A196" s="7">
         <v>43619.512569479164</v>
       </c>
@@ -9253,7 +9253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A197" s="7">
         <v>43619.559027557872</v>
       </c>
@@ -9282,7 +9282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A198" s="7">
         <v>43619.560911979162</v>
       </c>
@@ -9305,7 +9305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A199" s="7">
         <v>43619.580106157402</v>
       </c>
@@ -9334,7 +9334,7 @@
         <v>8500</v>
       </c>
     </row>
-    <row r="200" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A200" s="7">
         <v>43619.586162476851</v>
       </c>
@@ -9357,7 +9357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A201" s="7">
         <v>43619.593100185186</v>
       </c>
@@ -9389,7 +9389,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="202" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A202" s="7">
         <v>43619.603138240738</v>
       </c>
@@ -9418,7 +9418,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="203" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A203" s="7">
         <v>43619.624149479168</v>
       </c>
@@ -9447,7 +9447,7 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="204" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A204" s="7">
         <v>43619.636075578703</v>
       </c>
@@ -9479,7 +9479,7 @@
         <v>2820</v>
       </c>
     </row>
-    <row r="205" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A205" s="7">
         <v>43619.657319212958</v>
       </c>
@@ -9511,7 +9511,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="206" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A206" s="7">
         <v>43619.669281388888</v>
       </c>
@@ -9534,7 +9534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A207" s="7">
         <v>43619.683368090278</v>
       </c>
@@ -9566,7 +9566,7 @@
         <v>2220</v>
       </c>
     </row>
-    <row r="208" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A208" s="7">
         <v>43620.42668315972</v>
       </c>
@@ -9592,7 +9592,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="209" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A209" s="7">
         <v>43620.433715914347</v>
       </c>
@@ -9621,7 +9621,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="210" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A210" s="7">
         <v>43620.449795451394</v>
       </c>
@@ -9650,7 +9650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A211" s="7">
         <v>43620.468617280094</v>
       </c>
@@ -9694,7 +9694,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="212" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A212" s="7">
         <v>43620.486011516201</v>
       </c>
@@ -9735,7 +9735,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="213" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A213" s="7">
         <v>43620.487928645831</v>
       </c>
@@ -9764,7 +9764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A214" s="7">
         <v>43620.488378425929</v>
       </c>
@@ -9804,7 +9804,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="216" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A216" s="7">
         <v>43620.502757766204</v>
       </c>
@@ -9833,7 +9833,7 @@
         <v>8700</v>
       </c>
     </row>
-    <row r="217" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A217" s="7">
         <v>43620.503008993051</v>
       </c>
@@ -9874,7 +9874,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="218" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A218" s="7">
         <v>43620.516394976847</v>
       </c>
@@ -9900,7 +9900,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="219" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A219" s="7">
         <v>43620.531383842594</v>
       </c>
@@ -9923,7 +9923,7 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="220" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A220" s="7">
         <v>43620.534318229169</v>
       </c>
@@ -9952,7 +9952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A221" s="7">
         <v>43620.53862825231</v>
       </c>
@@ -9981,7 +9981,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="222" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A222" s="7">
         <v>43620.544621446759</v>
       </c>
@@ -10010,7 +10010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A223" s="7">
         <v>43620.559045000002</v>
       </c>
@@ -10051,7 +10051,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="224" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A224" s="7">
         <v>43620.562107916667</v>
       </c>
@@ -10074,7 +10074,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="225" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A225" s="7">
         <v>43620.57524528935</v>
       </c>
@@ -10115,7 +10115,7 @@
         <v>1540</v>
       </c>
     </row>
-    <row r="226" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A226" s="7">
         <v>43620.57848960648</v>
       </c>
@@ -10144,7 +10144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A227" s="7">
         <v>43620.589187465273</v>
       </c>
@@ -10167,7 +10167,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="228" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A228" s="7">
         <v>43620.646162557867</v>
       </c>
@@ -10208,7 +10208,7 @@
         <v>2215</v>
       </c>
     </row>
-    <row r="229" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A229" s="7">
         <v>43620.686772013883</v>
       </c>
@@ -10231,7 +10231,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="230" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A230" s="7">
         <v>43623.521720659723</v>
       </c>
@@ -10254,7 +10254,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="231" spans="1:15" s="22" customFormat="1" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:15" s="22" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A231" s="18">
         <v>43623.522309618056</v>
       </c>
@@ -11053,7 +11053,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="257" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" s="7">
         <v>43634.405545023154</v>
       </c>
@@ -12596,7 +12596,7 @@
       </c>
       <c r="Q302" s="5"/>
     </row>
-    <row r="303" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" s="7">
         <v>43647.44526699074</v>
       </c>
@@ -14401,7 +14401,7 @@
         <v>1830</v>
       </c>
     </row>
-    <row r="358" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A358" s="25">
         <v>43661.463808819448</v>
       </c>
@@ -14433,7 +14433,7 @@
         <v>5707</v>
       </c>
     </row>
-    <row r="359" spans="1:16" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A359" s="25">
         <v>43661.465437303239</v>
       </c>
@@ -14465,7 +14465,7 @@
         <v>2455</v>
       </c>
     </row>
-    <row r="360" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A360" s="25">
         <v>43661.470525659723</v>
       </c>
@@ -14494,7 +14494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="361" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A361" s="25">
         <v>43661.475225057875</v>
       </c>
@@ -14526,7 +14526,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="362" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A362" s="25">
         <v>43661.488394363427</v>
       </c>
@@ -14558,7 +14558,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="363" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A363" s="25">
         <v>43661.49257905093</v>
       </c>
@@ -14590,7 +14590,7 @@
         <v>1940</v>
       </c>
     </row>
-    <row r="364" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A364" s="25">
         <v>43661.496228148149</v>
       </c>
@@ -14622,7 +14622,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="365" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A365" s="25">
         <v>43661.502193263892</v>
       </c>
@@ -14654,7 +14654,7 @@
         <v>3342</v>
       </c>
     </row>
-    <row r="366" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A366" s="25">
         <v>43661.52084143518</v>
       </c>
@@ -14686,7 +14686,7 @@
         <v>1672</v>
       </c>
     </row>
-    <row r="367" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A367" s="25">
         <v>43661.539627453705</v>
       </c>
@@ -14718,7 +14718,7 @@
         <v>1442</v>
       </c>
     </row>
-    <row r="368" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A368" s="25">
         <v>43661.544727465276</v>
       </c>
@@ -14750,7 +14750,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="369" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A369" s="25">
         <v>43661.571753194439</v>
       </c>
@@ -14782,7 +14782,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="370" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A370" s="25">
         <v>43661.575824953703</v>
       </c>
@@ -14808,7 +14808,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="371" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A371" s="25">
         <v>43661.595967152782</v>
       </c>
@@ -14837,7 +14837,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="372" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A372" s="25">
         <v>43662.505582557875</v>
       </c>
@@ -14869,7 +14869,7 @@
         <v>4650</v>
       </c>
     </row>
-    <row r="373" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A373" s="25">
         <v>43662.403231944445</v>
       </c>
@@ -14901,7 +14901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="374" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A374" s="25">
         <v>43662.417311712961</v>
       </c>
@@ -14933,7 +14933,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="375" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A375" s="25">
         <v>43662.423942743058</v>
       </c>
@@ -14965,7 +14965,7 @@
         <v>3077</v>
       </c>
     </row>
-    <row r="376" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A376" s="25">
         <v>43662.43173575231</v>
       </c>
@@ -14994,7 +14994,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="377" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A377" s="25">
         <v>43662.438895104162</v>
       </c>
@@ -15023,7 +15023,7 @@
         <v>2620</v>
       </c>
     </row>
-    <row r="378" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A378" s="25">
         <v>43662.457425300927</v>
       </c>
@@ -15052,7 +15052,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="379" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A379" s="25">
         <v>43662.470728321758</v>
       </c>
@@ -15084,7 +15084,7 @@
         <v>1778</v>
       </c>
     </row>
-    <row r="380" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A380" s="25">
         <v>43662.481005601847</v>
       </c>
@@ -15116,7 +15116,7 @@
         <v>1844</v>
       </c>
     </row>
-    <row r="381" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A381" s="25">
         <v>43662.503588680556</v>
       </c>
@@ -15148,7 +15148,7 @@
         <v>1834</v>
       </c>
     </row>
-    <row r="382" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A382" s="25">
         <v>43662.508576585649</v>
       </c>
@@ -15180,7 +15180,7 @@
         <v>2690</v>
       </c>
     </row>
-    <row r="383" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A383" s="25">
         <v>43662.515664699073</v>
       </c>
@@ -15212,7 +15212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="384" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A384" s="25">
         <v>43662.523681469909</v>
       </c>
@@ -15244,7 +15244,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="385" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A385" s="25">
         <v>43662.524749976852</v>
       </c>
@@ -15276,7 +15276,7 @@
         <v>2651</v>
       </c>
     </row>
-    <row r="386" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A386" s="25">
         <v>43662.526702222225</v>
       </c>
@@ -15308,7 +15308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="387" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A387" s="25">
         <v>43662.528149259262</v>
       </c>
@@ -15338,7 +15338,7 @@
         <v>999999999</v>
       </c>
     </row>
-    <row r="388" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A388" s="25">
         <v>43662.530195763888</v>
       </c>
@@ -15370,7 +15370,7 @@
         <v>2690</v>
       </c>
     </row>
-    <row r="389" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A389" s="25">
         <v>43662.533871203705</v>
       </c>
@@ -15402,7 +15402,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="390" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A390" s="25">
         <v>43662.534038217593</v>
       </c>
@@ -15434,7 +15434,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="391" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A391" s="25">
         <v>43662.552655601852</v>
       </c>
@@ -15466,7 +15466,7 @@
         <v>1820</v>
       </c>
     </row>
-    <row r="392" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A392" s="25">
         <v>43662.553831041667</v>
       </c>
@@ -15498,7 +15498,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="393" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A393" s="25">
         <v>43662.553892222219</v>
       </c>
@@ -15527,7 +15527,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="394" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A394" s="25">
         <v>43662.576265393523</v>
       </c>
@@ -15556,7 +15556,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="395" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A395" s="25">
         <v>43662.605140277781</v>
       </c>
@@ -15588,7 +15588,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="396" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A396" s="25">
         <v>43662.608947546294</v>
       </c>
@@ -15617,7 +15617,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="397" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A397" s="25">
         <v>43662.630076076384</v>
       </c>
@@ -15640,7 +15640,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="398" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A398" s="25">
         <v>43662.638398935189</v>
       </c>
@@ -15669,7 +15669,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="399" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A399" s="25">
         <v>43662.651400266201</v>
       </c>
@@ -15698,7 +15698,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="400" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A400" s="25">
         <v>43662.653115231486</v>
       </c>
@@ -15727,7 +15727,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="401" spans="1:23" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:23" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A401" s="25">
         <v>43662.868660763888</v>
       </c>
@@ -15756,7 +15756,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="402" spans="1:23" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:23" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A402" s="25">
         <v>43665.537839201388</v>
       </c>
@@ -15785,7 +15785,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="403" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:23" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A403" s="25">
         <v>43665.538775069443</v>
       </c>
@@ -15808,7 +15808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="404" spans="1:23" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:23" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A404" s="25">
         <v>43665.565719756945</v>
       </c>
@@ -15837,7 +15837,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="405" spans="1:23" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:23" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A405" s="25">
         <v>43665.602270196759</v>
       </c>
@@ -16153,7 +16153,7 @@
       <c r="V412" s="36"/>
       <c r="W412" s="36"/>
     </row>
-    <row r="413" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A413" s="35">
         <v>43677.412245370368</v>
       </c>
@@ -16282,7 +16282,7 @@
       <c r="V415" s="36"/>
       <c r="W415" s="36"/>
     </row>
-    <row r="416" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A416" s="35">
         <v>43677.419004629628</v>
       </c>
@@ -18003,9 +18003,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:U454">
-    <filterColumn colId="1">
+    <filterColumn colId="2">
       <filters>
-        <filter val="SDR-204A"/>
+        <dateGroupItem year="2019" month="6" day="3" dateTimeGrouping="day"/>
+        <dateGroupItem year="2019" month="6" day="4" dateTimeGrouping="day"/>
+        <dateGroupItem year="2019" month="6" day="7" dateTimeGrouping="day"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
July op plan deliverable done
</commit_message>
<xml_diff>
--- a/0 - Field Data Sheets/Weir Calibration Field Form 2019 CURRENT 07_31_2019.xlsx
+++ b/0 - Field Data Sheets/Weir Calibration Field Form 2019 CURRENT 07_31_2019.xlsx
@@ -17,7 +17,7 @@
     <sheet name="ESRI_MAPINFO_SHEET" sheetId="3" state="veryHidden" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Form Responses 1'!$A$1:$U$454</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Form Responses 1'!$A$1:$W$454</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -108,6 +108,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Responder updated this value.</t>
         </r>
@@ -1752,18 +1753,21 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2310,8 +2314,8 @@
   <dimension ref="A1:W454"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A194" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B218" sqref="B218"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G277" sqref="G277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3632,7 +3636,7 @@
       </c>
       <c r="J42" s="5"/>
     </row>
-    <row r="43" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>43592.691540694446</v>
       </c>
@@ -3781,7 +3785,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <v>43593.460052071758</v>
       </c>
@@ -5632,7 +5636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A95" s="7">
         <v>43594.908273356486</v>
       </c>
@@ -6631,7 +6635,7 @@
         <v>2430</v>
       </c>
     </row>
-    <row r="122" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A122" s="7">
         <v>43595.588972465281</v>
       </c>
@@ -8881,7 +8885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="7">
         <v>43619.417066539347</v>
       </c>
@@ -8910,7 +8914,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="186" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="7">
         <v>43619.424325891203</v>
       </c>
@@ -8945,7 +8949,7 @@
         <v>8600</v>
       </c>
     </row>
-    <row r="187" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="7">
         <v>43619.430370590278</v>
       </c>
@@ -8974,7 +8978,7 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="188" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="7">
         <v>43619.448148344905</v>
       </c>
@@ -8997,7 +9001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="7">
         <v>43619.449386782406</v>
       </c>
@@ -9041,7 +9045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="7">
         <v>43619.457925891205</v>
       </c>
@@ -9085,7 +9089,7 @@
         <v>4910</v>
       </c>
     </row>
-    <row r="191" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="7">
         <v>43619.481042361112</v>
       </c>
@@ -9114,7 +9118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="7">
         <v>43619.482240219906</v>
       </c>
@@ -9143,7 +9147,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="193" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="7">
         <v>43619.485708449072</v>
       </c>
@@ -9172,7 +9176,7 @@
         <v>2470</v>
       </c>
     </row>
-    <row r="194" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="7">
         <v>43619.502512523148</v>
       </c>
@@ -9201,7 +9205,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="195" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="7">
         <v>43619.50333712963</v>
       </c>
@@ -9224,7 +9228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="7">
         <v>43619.512569479164</v>
       </c>
@@ -9253,7 +9257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="7">
         <v>43619.559027557872</v>
       </c>
@@ -9282,7 +9286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="7">
         <v>43619.560911979162</v>
       </c>
@@ -9305,7 +9309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="7">
         <v>43619.580106157402</v>
       </c>
@@ -9334,7 +9338,7 @@
         <v>8500</v>
       </c>
     </row>
-    <row r="200" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="7">
         <v>43619.586162476851</v>
       </c>
@@ -9357,7 +9361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="7">
         <v>43619.593100185186</v>
       </c>
@@ -9389,7 +9393,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="202" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="7">
         <v>43619.603138240738</v>
       </c>
@@ -9418,7 +9422,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="203" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="7">
         <v>43619.624149479168</v>
       </c>
@@ -9447,7 +9451,7 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="204" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="7">
         <v>43619.636075578703</v>
       </c>
@@ -9479,7 +9483,7 @@
         <v>2820</v>
       </c>
     </row>
-    <row r="205" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="7">
         <v>43619.657319212958</v>
       </c>
@@ -9511,7 +9515,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="206" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="7">
         <v>43619.669281388888</v>
       </c>
@@ -9534,7 +9538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="7">
         <v>43619.683368090278</v>
       </c>
@@ -9566,7 +9570,7 @@
         <v>2220</v>
       </c>
     </row>
-    <row r="208" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:11" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="7">
         <v>43620.42668315972</v>
       </c>
@@ -9592,7 +9596,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="209" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="7">
         <v>43620.433715914347</v>
       </c>
@@ -9621,7 +9625,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="210" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="7">
         <v>43620.449795451394</v>
       </c>
@@ -9650,7 +9654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="7">
         <v>43620.468617280094</v>
       </c>
@@ -9694,7 +9698,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="212" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="7">
         <v>43620.486011516201</v>
       </c>
@@ -9735,7 +9739,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="213" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="7">
         <v>43620.487928645831</v>
       </c>
@@ -9764,7 +9768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="7">
         <v>43620.488378425929</v>
       </c>
@@ -9784,7 +9788,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="215" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="7">
         <v>43620.488762453708</v>
       </c>
@@ -9804,7 +9808,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="216" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="7">
         <v>43620.502757766204</v>
       </c>
@@ -9833,7 +9837,7 @@
         <v>8700</v>
       </c>
     </row>
-    <row r="217" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="7">
         <v>43620.503008993051</v>
       </c>
@@ -9874,7 +9878,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="218" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="7">
         <v>43620.516394976847</v>
       </c>
@@ -9900,7 +9904,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="219" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="7">
         <v>43620.531383842594</v>
       </c>
@@ -9923,7 +9927,7 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="220" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="7">
         <v>43620.534318229169</v>
       </c>
@@ -9952,7 +9956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="7">
         <v>43620.53862825231</v>
       </c>
@@ -9981,7 +9985,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="222" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="7">
         <v>43620.544621446759</v>
       </c>
@@ -10010,7 +10014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="7">
         <v>43620.559045000002</v>
       </c>
@@ -10051,7 +10055,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="224" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="7">
         <v>43620.562107916667</v>
       </c>
@@ -10115,7 +10119,7 @@
         <v>1540</v>
       </c>
     </row>
-    <row r="226" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="7">
         <v>43620.57848960648</v>
       </c>
@@ -10144,7 +10148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="7">
         <v>43620.589187465273</v>
       </c>
@@ -10167,7 +10171,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="228" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="7">
         <v>43620.646162557867</v>
       </c>
@@ -10208,7 +10212,7 @@
         <v>2215</v>
       </c>
     </row>
-    <row r="229" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="7">
         <v>43620.686772013883</v>
       </c>
@@ -10231,7 +10235,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="230" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="7">
         <v>43623.521720659723</v>
       </c>
@@ -10254,7 +10258,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="231" spans="1:15" s="22" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:15" s="22" customFormat="1" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="18">
         <v>43623.522309618056</v>
       </c>
@@ -11654,7 +11658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A277" s="7">
         <v>43634.51392675926</v>
       </c>
@@ -11686,7 +11690,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="278" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A278" s="7">
         <v>43634.530469999998</v>
       </c>
@@ -13981,7 +13985,7 @@
       </c>
       <c r="Q344" s="5"/>
     </row>
-    <row r="345" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A345" s="7">
         <v>43648.574154016205</v>
       </c>
@@ -15402,7 +15406,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="390" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:16" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A390" s="25">
         <v>43662.534038217593</v>
       </c>
@@ -15698,7 +15702,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="400" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A400" s="25">
         <v>43662.653115231486</v>
       </c>
@@ -15727,7 +15731,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="401" spans="1:23" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A401" s="25">
         <v>43662.868660763888</v>
       </c>
@@ -15837,7 +15841,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="405" spans="1:23" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A405" s="25">
         <v>43665.602270196759</v>
       </c>
@@ -17463,7 +17467,7 @@
       <c r="V442" s="36"/>
       <c r="W442" s="36"/>
     </row>
-    <row r="443" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A443" s="35">
         <v>43678.404270833336</v>
       </c>
@@ -18002,12 +18006,10 @@
       <c r="W454" s="43"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U454">
-    <filterColumn colId="2">
+  <autoFilter ref="A1:W454">
+    <filterColumn colId="1">
       <filters>
-        <dateGroupItem year="2019" month="6" day="3" dateTimeGrouping="day"/>
-        <dateGroupItem year="2019" month="6" day="4" dateTimeGrouping="day"/>
-        <dateGroupItem year="2019" month="6" day="7" dateTimeGrouping="day"/>
+        <filter val="SDG-084"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>